<commit_message>
starting exploratory analysis for the dataset
</commit_message>
<xml_diff>
--- a/agent-based-basic/dataset_description.xlsx
+++ b/agent-based-basic/dataset_description.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10908"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/giuliatesta/PycharmProjects/masters-thesis-project/agent-based-basic/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FD292258-D341-0A4C-8970-3B7F44813ED1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E8A3B13-0928-C847-8A63-195088CF8DBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{C5BC5EF6-5451-B047-9842-11FEED8FA920}"/>
+    <workbookView xWindow="-20" yWindow="500" windowWidth="28800" windowHeight="16000" xr2:uid="{C5BC5EF6-5451-B047-9842-11FEED8FA920}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="description" localSheetId="0">Sheet1!$A$1:$AT$5</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -711,10 +711,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19EC5248-E578-3F48-B655-2FD1E8F005C7}">
-  <dimension ref="A1:AT5"/>
+  <dimension ref="A1:AT6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="E4" sqref="E4:E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -722,8 +722,8 @@
     <col min="1" max="1" width="6.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="5.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.1640625" customWidth="1"/>
+    <col min="5" max="5" width="11.5" customWidth="1"/>
     <col min="6" max="6" width="34.33203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="6.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="19.6640625" bestFit="1" customWidth="1"/>
@@ -1461,6 +1461,188 @@
         <v>3</v>
       </c>
     </row>
+    <row r="6" spans="1:46" x14ac:dyDescent="0.2">
+      <c r="B6">
+        <f>B5/B2 * 100</f>
+        <v>1.9592476489028211E-2</v>
+      </c>
+      <c r="C6">
+        <f t="shared" ref="C6:M6" si="0">C5/C2 * 100</f>
+        <v>1.9592476489028211E-2</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>6.7398119122257061</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="0"/>
+        <v>50.372257053291534</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="0"/>
+        <v>48.824451410658313</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="0"/>
+        <v>2.3706896551724137</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="0"/>
+        <v>19.455329153605017</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="0"/>
+        <v>64.439655172413794</v>
+      </c>
+      <c r="J6">
+        <f t="shared" si="0"/>
+        <v>27.605799373040753</v>
+      </c>
+      <c r="K6">
+        <f t="shared" si="0"/>
+        <v>53.957680250783703</v>
+      </c>
+      <c r="L6">
+        <f t="shared" si="0"/>
+        <v>51.391065830721004</v>
+      </c>
+      <c r="M6">
+        <f t="shared" si="0"/>
+        <v>50.528996865203759</v>
+      </c>
+      <c r="N6">
+        <f>N5/N2 * 100</f>
+        <v>54.839341692789965</v>
+      </c>
+      <c r="O6">
+        <f t="shared" ref="O6" si="1">O5/O2 * 100</f>
+        <v>75.391849529780558</v>
+      </c>
+      <c r="P6">
+        <f t="shared" ref="P6" si="2">P5/P2 * 100</f>
+        <v>49.529780564263319</v>
+      </c>
+      <c r="Q6">
+        <f t="shared" ref="Q6:R6" si="3">Q5/Q2 * 100</f>
+        <v>29.584639498432601</v>
+      </c>
+      <c r="R6">
+        <f t="shared" si="3"/>
+        <v>50.607366771159882</v>
+      </c>
+      <c r="S6">
+        <f t="shared" ref="S6" si="4">S5/S2 * 100</f>
+        <v>50.411442006269588</v>
+      </c>
+      <c r="T6">
+        <f t="shared" ref="T6" si="5">T5/T2 * 100</f>
+        <v>58.836206896551722</v>
+      </c>
+      <c r="U6">
+        <f t="shared" ref="U6" si="6">U5/U2 * 100</f>
+        <v>68.123040752351088</v>
+      </c>
+      <c r="V6">
+        <f t="shared" ref="V6" si="7">V5/V2 * 100</f>
+        <v>53.017241379310342</v>
+      </c>
+      <c r="W6">
+        <f t="shared" ref="W6" si="8">W5/W2 * 100</f>
+        <v>67.06504702194357</v>
+      </c>
+      <c r="X6">
+        <f t="shared" ref="X6" si="9">X5/X2 * 100</f>
+        <v>82.601880877742957</v>
+      </c>
+      <c r="Y6">
+        <f t="shared" ref="Y6" si="10">Y5/Y2 * 100</f>
+        <v>82.719435736677113</v>
+      </c>
+      <c r="Z6">
+        <f t="shared" ref="Z6" si="11">Z5/Z2 * 100</f>
+        <v>82.307993730407532</v>
+      </c>
+      <c r="AA6">
+        <f t="shared" ref="AA6" si="12">AA5/AA2 * 100</f>
+        <v>51.038401253918494</v>
+      </c>
+      <c r="AB6">
+        <f t="shared" ref="AB6" si="13">AB5/AB2 * 100</f>
+        <v>94.083072100313487</v>
+      </c>
+      <c r="AC6">
+        <f t="shared" ref="AC6:AD6" si="14">AC5/AC2 * 100</f>
+        <v>51.626175548589337</v>
+      </c>
+      <c r="AD6">
+        <f t="shared" si="14"/>
+        <v>64.831504702194351</v>
+      </c>
+      <c r="AE6">
+        <f t="shared" ref="AE6" si="15">AE5/AE2 * 100</f>
+        <v>46.590909090909086</v>
+      </c>
+      <c r="AF6">
+        <f t="shared" ref="AF6" si="16">AF5/AF2 * 100</f>
+        <v>23.824451410658305</v>
+      </c>
+      <c r="AG6">
+        <f t="shared" ref="AG6:AH6" si="17">AG5/AG2 * 100</f>
+        <v>23.687304075235112</v>
+      </c>
+      <c r="AH6">
+        <f t="shared" si="17"/>
+        <v>29.956896551724139</v>
+      </c>
+      <c r="AI6">
+        <f t="shared" ref="AI6" si="18">AI5/AI2 * 100</f>
+        <v>32.464733542319749</v>
+      </c>
+      <c r="AJ6">
+        <f t="shared" ref="AJ6" si="19">AJ5/AJ2 * 100</f>
+        <v>32.112068965517246</v>
+      </c>
+      <c r="AK6">
+        <f t="shared" ref="AK6" si="20">AK5/AK2 * 100</f>
+        <v>50.411442006269588</v>
+      </c>
+      <c r="AL6">
+        <f t="shared" ref="AL6" si="21">AL5/AL2 * 100</f>
+        <v>48.824451410658313</v>
+      </c>
+      <c r="AM6">
+        <f t="shared" ref="AM6" si="22">AM5/AM2 * 100</f>
+        <v>53.957680250783703</v>
+      </c>
+      <c r="AN6">
+        <f t="shared" ref="AN6" si="23">AN5/AN2 * 100</f>
+        <v>19.455329153605017</v>
+      </c>
+      <c r="AO6">
+        <f t="shared" ref="AO6" si="24">AO5/AO2 * 100</f>
+        <v>32.112068965517246</v>
+      </c>
+      <c r="AP6">
+        <f t="shared" ref="AP6" si="25">AP5/AP2 * 100</f>
+        <v>29.584639498432601</v>
+      </c>
+      <c r="AQ6">
+        <f t="shared" ref="AQ6" si="26">AQ5/AQ2 * 100</f>
+        <v>23.687304075235112</v>
+      </c>
+      <c r="AR6">
+        <f t="shared" ref="AR6" si="27">AR5/AR2 * 100</f>
+        <v>6.7398119122257061</v>
+      </c>
+      <c r="AS6">
+        <f t="shared" ref="AS6:AT6" si="28">AS5/AS2 * 100</f>
+        <v>5.8777429467084641E-2</v>
+      </c>
+      <c r="AT6">
+        <f t="shared" si="28"/>
+        <v>5.8777429467084641E-2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>